<commit_message>
Modify Ssld examplar and Free reporting section
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssld_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssld_vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD4588A-B267-4F88-A6F8-A2C277E0F161}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB148119-E390-4507-B5EF-93E8B05F8E3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="32760" windowHeight="17145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>A</t>
   </si>
@@ -92,9 +92,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Auflösung</t>
-  </si>
-  <si>
     <t>Manuell</t>
   </si>
   <si>
@@ -182,6 +179,12 @@
   <si>
     <t>PZB-
 Schutzpunkt</t>
+  </si>
+  <si>
+    <t>Auflösung (im Zielgleis)</t>
+  </si>
+  <si>
+    <t>Bemessungslänge</t>
   </si>
 </sst>
 </file>
@@ -555,28 +558,28 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -940,11 +943,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:U63"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C1" zoomScale="175" zoomScaleNormal="100" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -962,7 +965,8 @@
     <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" style="1" customWidth="1"/>
     <col min="20" max="20" width="11.42578125" style="3"/>
     <col min="21" max="21" width="45.42578125" style="18" customWidth="1"/>
     <col min="22" max="16384" width="11.42578125" style="3"/>
@@ -1018,113 +1022,113 @@
         <v>20</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="38"/>
       <c r="D2" s="38"/>
       <c r="E2" s="39"/>
       <c r="F2" s="40"/>
       <c r="G2" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="38"/>
       <c r="I2" s="38"/>
       <c r="J2" s="38"/>
       <c r="K2" s="40"/>
       <c r="L2" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
       <c r="O2" s="38"/>
       <c r="P2" s="40"/>
       <c r="Q2" s="41" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="R2" s="42"/>
       <c r="S2" s="42"/>
       <c r="T2" s="43"/>
-      <c r="U2" s="29" t="s">
-        <v>42</v>
+      <c r="U2" s="34" t="s">
+        <v>41</v>
       </c>
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" s="5" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" s="30"/>
+      <c r="Q3" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="30"/>
+      <c r="T3" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="35"/>
     </row>
     <row r="4" spans="1:22" s="8" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="32"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1132,27 +1136,27 @@
         <v>8</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="36"/>
+        <v>45</v>
+      </c>
+      <c r="K4" s="33"/>
       <c r="L4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="32"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="36"/>
       <c r="R4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="T4" s="36"/>
-      <c r="U4" s="30"/>
+        <v>49</v>
+      </c>
+      <c r="T4" s="33"/>
+      <c r="U4" s="35"/>
     </row>
     <row r="5" spans="1:22" s="16" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -1162,19 +1166,19 @@
       <c r="E5" s="11"/>
       <c r="F5" s="12"/>
       <c r="G5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="L5" s="14"/>
       <c r="M5" s="13"/>
@@ -1184,10 +1188,10 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="T5" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="U5" s="17"/>
     </row>
@@ -2525,16 +2529,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="U2:U4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E3:E4"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="L2:P2"/>
@@ -2545,6 +2539,16 @@
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:K4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="U2:U4"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.19685039370078741" bottom="0.59055118110236227" header="0" footer="0"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -2598,19 +2602,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -2802,6 +2793,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
   <ds:schemaRefs>
@@ -2811,22 +2815,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947F1741-2986-4B63-8B5C-D0468C671233}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD45C59E-C13E-4B92-9551-AE1790848EFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2843,4 +2831,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947F1741-2986-4B63-8B5C-D0468C671233}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>